<commit_message>
this second face book
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15960" windowHeight="6420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11895" windowHeight="6165" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1:N12"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:F19"/>
 </workbook>
 </file>
 
@@ -49,14 +49,14 @@
     <t>Photo Add</t>
   </si>
   <si>
-    <t>D:\ganesha fest\IMG_0007.JPG</t>
+    <t>F:\GraphicsViewer.aspx.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +107,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -185,6 +190,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -219,6 +225,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,20 +401,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -433,29 +440,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -466,20 +473,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -487,7 +494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>

</xml_diff>